<commit_message>
Added Large 1000W codes + IR Sketch document
</commit_message>
<xml_diff>
--- a/Projectors IR Codes.xlsx
+++ b/Projectors IR Codes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Naseem\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB1FF5BD-9213-4362-8E56-85FEDC7B8E2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{395DBB8B-C740-4326-8781-6B7E4B9F9399}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{F431D6CF-0187-45AC-832C-6CAA98B7F692}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{F431D6CF-0187-45AC-832C-6CAA98B7F692}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="84">
   <si>
     <t>Big Projector</t>
   </si>
@@ -245,6 +245,51 @@
   </si>
   <si>
     <t>0x1FE906F</t>
+  </si>
+  <si>
+    <t>uint16_t rawData[67] = {9014, 4486,  582, 544,  584, 544,  584, 546,  558, 570,  558, 570,  558, 568,  584, 544,  584, 1648,  582, 1648,  584, 1648,  582, 1648,  582, 1646,  584, 1648,  558, 1672,  562, 1672,  580, 544,  586, 1646,  584, 546,  582, 546,  558, 570,  558, 572,  580, 548,  580, 546,  580, 548,  556, 572,  556, 1674,  556, 1676,  554, 1676,  554, 1676,  552, 1678,  552, 1678,  552, 1680,  552};  // NEC 1FE807F</t>
+  </si>
+  <si>
+    <t>Full Brightness</t>
+  </si>
+  <si>
+    <t>Code      : 0x1FE609F (32 Bits)</t>
+  </si>
+  <si>
+    <t>uint16_t rawData[67] = {9020, 4480,  586, 544,  584, 544,  584, 542,  586, 542,  588, 542,  586, 544,  584, 542,  584, 1646,  586, 1646,  584, 1644,  584, 1646,  584, 1646,  586, 1644,  586, 1646,  584, 1644,  586, 544,  582, 546,  584, 1646,  582, 1648,  584, 546,  582, 546,  582, 546,  582, 546,  558, 570,  582, 1646,  584, 546,  582, 546,  580, 1650,  580, 1648,  580, 1650,  556, 1674,  580, 1650,  578};  // NEC 1FE609F</t>
+  </si>
+  <si>
+    <t>uint32_t command = 0x6;</t>
+  </si>
+  <si>
+    <t>uint64_t data = 0x1FE609F;</t>
+  </si>
+  <si>
+    <t>Half Brightness</t>
+  </si>
+  <si>
+    <t>Code      : 0x1FEA05F (32 Bits)</t>
+  </si>
+  <si>
+    <t>uint16_t rawData[67] = {9020, 4478,  586, 544,  586, 544,  584, 542,  586, 542,  586, 544,  584, 544,  580, 548,  560, 1670,  586, 1644,  588, 1644,  586, 1644,  586, 1646,  562, 1666,  586, 1644,  584, 1646,  584, 544,  582, 1648,  556, 572,  556, 1674,  556, 572,  556, 572,  556, 572,  556, 574,  554, 574,  554, 574,  552, 1678,  552, 576,  552, 1678,  550, 1678,  552, 1678,  552, 1680,  550, 1680,  550};  // NEC 1FEA05F</t>
+  </si>
+  <si>
+    <t>uint32_t command = 0x5;</t>
+  </si>
+  <si>
+    <t>uint64_t data = 0x1FEA05F;</t>
+  </si>
+  <si>
+    <t>Always</t>
+  </si>
+  <si>
+    <t>uint16_t rawData[67] = {9026, 4480,  588, 540,  588, 544,  586, 542,  586, 542,  562, 566,  562, 566,  562, 566,  584, 1646,  584, 1646,  586, 1644,  588, 1644,  588, 1642,  586, 1644,  562, 1668,  584, 1646,  562, 592,  536, 572,  556, 1672,  560, 1672,  558, 1674,  556, 1674,  556, 596,  532, 596,  532, 598,  530, 1678,  554, 598,  530, 598,  528, 600,  530, 598,  528, 1680,  550, 1704,  526, 1704,  528};  // NEC 1FE7887</t>
+  </si>
+  <si>
+    <t>0x1FE609F</t>
+  </si>
+  <si>
+    <t>0x1FEA05F</t>
   </si>
 </sst>
 </file>
@@ -1083,7 +1128,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EB5D0BE-9A24-49CF-A0DC-E6997873318A}">
   <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
@@ -1246,15 +1291,17 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D238925F-06AA-4444-85DE-E12009D07106}">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="3" width="26.5546875" customWidth="1"/>
+    <col min="1" max="1" width="13.5546875" customWidth="1"/>
+    <col min="2" max="2" width="26.5546875" customWidth="1"/>
+    <col min="3" max="3" width="26.5546875" style="2" customWidth="1"/>
     <col min="4" max="4" width="16.5546875" customWidth="1"/>
     <col min="5" max="5" width="29.33203125" customWidth="1"/>
   </cols>
@@ -1266,7 +1313,7 @@
       <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="4" t="s">
         <v>16</v>
       </c>
       <c r="D1" s="1" t="s">
@@ -1274,6 +1321,174 @@
       </c>
       <c r="E1" s="1" t="s">
         <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="2">
+        <v>33456255</v>
+      </c>
+      <c r="D3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E7" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E8" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>70</v>
+      </c>
+      <c r="B11" t="s">
+        <v>82</v>
+      </c>
+      <c r="C11" s="2">
+        <v>33448095</v>
+      </c>
+      <c r="D11" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E12" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E13" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E14" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E15" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E16" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>75</v>
+      </c>
+      <c r="B19" t="s">
+        <v>83</v>
+      </c>
+      <c r="C19" s="2">
+        <v>33464415</v>
+      </c>
+      <c r="D19" t="s">
+        <v>6</v>
+      </c>
+      <c r="E19" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E20" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E21" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E22" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E23" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E24" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>80</v>
+      </c>
+      <c r="B27" t="s">
+        <v>11</v>
+      </c>
+      <c r="C27" s="2">
+        <v>33454215</v>
+      </c>
+      <c r="D27" t="s">
+        <v>6</v>
+      </c>
+      <c r="E27" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E28" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E29" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E30" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E31" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E32" t="s">
+        <v>66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>